<commit_message>
fix: template delete work city field
--bug=1055850 --user=王旭 【系统】组织架构-导入-工作城市-导入后不显示 https://www.tapd.cn/34675357/s/1697357
</commit_message>
<xml_diff>
--- a/frontend/packages/web/public/templates/user_import_en.xlsx
+++ b/frontend/packages/web/public/templates/user_import_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\crm\cordys-crm\frontend\packages\web\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A179DD-E562-4911-A920-19E88767D9C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B2996E4-C32A-4F2F-8977-24A30C6FF057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6675" yWindow="1800" windowWidth="30750" windowHeight="17955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8055" yWindow="2880" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <author>admin</author>
   </authors>
   <commentList>
-    <comment ref="J3" authorId="0" shapeId="0" xr:uid="{6F5E1CB7-1B07-4953-837B-C98F3028ECE9}">
+    <comment ref="I3" authorId="0" shapeId="0" xr:uid="{6F5E1CB7-1B07-4953-837B-C98F3028ECE9}">
       <text>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Name</t>
   </si>
@@ -77,10 +77,6 @@
   </si>
   <si>
     <t>Phone</t>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <t>Work city</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
   <si>
@@ -201,14 +197,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -488,10 +484,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -500,7 +496,7 @@
     <col min="3" max="3" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="18.95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -512,25 +508,23 @@
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
+    <row r="2" spans="1:9" ht="36.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>0</v>
@@ -538,7 +532,7 @@
       <c r="C3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -551,18 +545,15 @@
         <v>3</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A2:I2"/>
   </mergeCells>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>